<commit_message>
added Emploi.xml and creation function
</commit_message>
<xml_diff>
--- a/FichiersExcel/Modules.xlsx
+++ b/FichiersExcel/Modules.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AnasChatt\Desktop\XMLProjet\Fichiers Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AnasChatt\Desktop\XMLProjet\FichiersExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D174FB43-68D7-43DE-80E6-46E05BF910D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B5E282-BA97-44D0-B1BB-AFD52B60C481}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{326FD6D2-A0C3-41BC-AF6A-CE3096327355}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{326FD6D2-A0C3-41BC-AF6A-CE3096327355}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -174,30 +174,6 @@
     <t>responsable</t>
   </si>
   <si>
-    <t>Mohamed El Haddad</t>
-  </si>
-  <si>
-    <t>Saida Rahali El Azzouzi</t>
-  </si>
-  <si>
-    <t>El Alami</t>
-  </si>
-  <si>
-    <t>Hassan Badir</t>
-  </si>
-  <si>
-    <t>Khalid Amechnoue</t>
-  </si>
-  <si>
-    <t>Amal Zaamouni</t>
-  </si>
-  <si>
-    <t>Ezzine</t>
-  </si>
-  <si>
-    <t>Lazaar</t>
-  </si>
-  <si>
     <t>semestre</t>
   </si>
   <si>
@@ -337,6 +313,30 @@
   </si>
   <si>
     <t>Projet collectif et stage</t>
+  </si>
+  <si>
+    <t>EL HADDAD</t>
+  </si>
+  <si>
+    <t>RAHALI EL AZZOUZI</t>
+  </si>
+  <si>
+    <t>EL ALAMI</t>
+  </si>
+  <si>
+    <t>BADIR</t>
+  </si>
+  <si>
+    <t>AMECHNOUE</t>
+  </si>
+  <si>
+    <t>ZAAMOUMI</t>
+  </si>
+  <si>
+    <t>EZZINE</t>
+  </si>
+  <si>
+    <t>LAZAAR</t>
   </si>
 </sst>
 </file>
@@ -736,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B328047C-6353-4DE4-AE9C-47238ED072FE}">
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -759,31 +759,31 @@
         <v>47</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>48</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -791,22 +791,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="D2" s="1">
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>39</v>
@@ -819,28 +819,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="D3" s="1">
         <v>3</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>28</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>33</v>
@@ -851,28 +851,28 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="D4" s="1">
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>29</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>30</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="J4" s="4" t="s">
         <v>46</v>
@@ -886,25 +886,25 @@
         <v>6</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>52</v>
+        <v>99</v>
       </c>
       <c r="D5" s="1">
         <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>34</v>
@@ -918,19 +918,19 @@
         <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
       <c r="D6" s="1">
         <v>3</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>31</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>32</v>
@@ -946,25 +946,25 @@
         <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>54</v>
+        <v>101</v>
       </c>
       <c r="D7" s="1">
         <v>3</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>38</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="J7" s="2" t="s">
         <v>35</v>
@@ -978,19 +978,19 @@
         <v>25</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="D8" s="1">
         <v>4</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>45</v>
@@ -1003,28 +1003,28 @@
         <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>52</v>
       </c>
       <c r="D9" s="1">
         <v>4</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>36</v>
@@ -1038,25 +1038,25 @@
         <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>55</v>
+        <v>102</v>
       </c>
       <c r="D10" s="1">
         <v>4</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>19</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>37</v>
@@ -1070,19 +1070,19 @@
         <v>40</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>51</v>
+        <v>98</v>
       </c>
       <c r="D11" s="1">
         <v>4</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>42</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>21</v>
@@ -1095,22 +1095,22 @@
         <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>56</v>
+        <v>103</v>
       </c>
       <c r="D12" s="1">
         <v>4</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>43</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>44</v>
@@ -1126,28 +1126,28 @@
         <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>49</v>
+        <v>96</v>
       </c>
       <c r="D13" s="1">
         <v>4</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>